<commit_message>
added assignment problem for matching gt and ft
</commit_message>
<xml_diff>
--- a/output_MTMM.xlsx
+++ b/output_MTMM.xlsx
@@ -340,21 +340,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -392,16 +392,19 @@
       <c r="O1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -437,18 +440,21 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -486,8 +492,11 @@
       <c r="O3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>0</v>
       </c>
@@ -501,10 +510,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -533,8 +542,11 @@
       <c r="O4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>0</v>
       </c>
@@ -548,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -578,10 +590,13 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>0</v>
       </c>
@@ -595,10 +610,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -625,10 +640,13 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>0</v>
       </c>
@@ -651,10 +669,10 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -674,8 +692,11 @@
       <c r="O7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>0</v>
       </c>
@@ -698,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -719,10 +740,13 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>0</v>
       </c>
@@ -745,10 +769,10 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -766,10 +790,13 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>0</v>
       </c>
@@ -798,13 +825,13 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -815,8 +842,11 @@
       <c r="O10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>0</v>
       </c>
@@ -848,10 +878,10 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -860,10 +890,13 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>0</v>
       </c>
@@ -895,10 +928,10 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -907,10 +940,13 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>0</v>
       </c>
@@ -951,13 +987,16 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>0</v>
       </c>
@@ -998,57 +1037,113 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B15">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>54</v>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>